<commit_message>
Implementando Layout do DashBoard
</commit_message>
<xml_diff>
--- a/Sales-Dashboard-3_0.xlsx
+++ b/Sales-Dashboard-3_0.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c548d412d6f19400/Área de Trabalho/Alura/excel/Projetos Youtube/03. DashVendas 3.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="468" documentId="13_ncr:1_{BFF51C44-DCD2-4F0A-BAAC-D0ADC01F5A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB22228E-4EEB-4CAC-A3E5-CA6DFF5761F7}"/>
+  <xr:revisionPtr revIDLastSave="476" documentId="13_ncr:1_{BFF51C44-DCD2-4F0A-BAAC-D0ADC01F5A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC510DAB-685D-4D64-8FCE-30EF3AF606FA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0A0D8D68-EFC2-4074-BDCA-85DAF874A3F1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{0A0D8D68-EFC2-4074-BDCA-85DAF874A3F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="3" r:id="rId1"/>
-    <sheet name="Input Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Master Data" sheetId="1" r:id="rId3"/>
+    <sheet name="Dashboard" sheetId="4" r:id="rId2"/>
+    <sheet name="Input Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Master Data" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Analysis!$AF$3:$AF$7</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Analysis!$AG$3:$AG$7</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Analysis!$AF$3:$AF$7</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Analysis!$AG$3:$AG$7</definedName>
     <definedName name="Category">OFFSET(Analysis!$AC$2,1,0,COUNT(Analysis!$AD:$AD))</definedName>
     <definedName name="CategoryRange">OFFSET(Analysis!$AC$2,1,1,COUNT(Analysis!$AD:$AD))</definedName>
     <definedName name="SegmentaçãodeDados_Month">#N/A</definedName>
@@ -31,15 +30,15 @@
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId5"/>
         <x14:slicerCache r:id="rId6"/>
         <x14:slicerCache r:id="rId7"/>
         <x14:slicerCache r:id="rId8"/>
+        <x14:slicerCache r:id="rId9"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -62,7 +61,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -496,9 +495,9 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="168" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,11 +519,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -594,7 +588,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -618,8 +612,7 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -629,9 +622,6 @@
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="30">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -837,6 +827,9 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     </dxf>
     <dxf>
       <font>
@@ -1703,7 +1696,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1737,7 +1729,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1771,7 +1762,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1805,7 +1795,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1839,7 +1828,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1873,7 +1861,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1907,7 +1894,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1941,7 +1927,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1975,7 +1960,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2009,7 +1993,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2043,7 +2026,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2077,7 +2059,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3038,6 +3019,48 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -3071,6 +3094,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-9824-48E2-B6D6-4EF765EB7C58}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -3086,6 +3114,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-9824-48E2-B6D6-4EF765EB7C58}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -3386,6 +3419,34 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -3419,6 +3480,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-5D90-41B6-A557-65439EEC999B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -3434,6 +3500,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-5D90-41B6-A557-65439EEC999B}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -7032,7 +7103,7 @@
             <xdr:cNvPr id="11" name="SALE TYPE">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EA923E7-5A58-8E5A-2425-3F07F67FC2EE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7110,7 +7181,7 @@
             <xdr:cNvPr id="12" name="PAYMENT MODE">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7125C087-C9B3-30C1-08B9-08253D7D90CD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7188,7 +7259,7 @@
             <xdr:cNvPr id="14" name="Month">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2462C4A-755D-A26D-646B-ADAC37F54D1E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7266,7 +7337,7 @@
             <xdr:cNvPr id="13" name="Year">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A864B697-2C8D-2192-9098-89FB887BB154}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7342,7 +7413,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54F31485-CABF-E5DC-3285-A8324B25EF0A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7378,7 +7449,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFF461BB-6196-FC1A-D0CF-E79264968990}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7401,13 +7472,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>786092</xdr:colOff>
+          <xdr:colOff>790575</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>224119</xdr:colOff>
+          <xdr:colOff>228600</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -7468,15 +7539,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>578223</xdr:colOff>
+          <xdr:colOff>581025</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>176493</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>11205</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>186018</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7486,7 +7557,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF84F5C3-644D-D0F4-47E4-1E34197F8CF3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7537,13 +7608,13 @@
           <xdr:col>10</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>183216</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
           <xdr:colOff>533400</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>2241</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7553,7 +7624,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17205045-7779-D049-86F3-185A756A6E70}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7615,7 +7686,7 @@
         <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7154606A-C59D-E44B-86D2-4C8F00C309F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7703,7 +7774,7 @@
             <xdr:cNvPr id="5" name="Gráfico 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07E146C2-436E-C12A-F30B-790BBEF1EB60}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7730,8 +7801,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="31623000" y="1592354"/>
-              <a:ext cx="3137647" cy="3562351"/>
+              <a:off x="31582099" y="1592354"/>
+              <a:ext cx="3134285" cy="3562351"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -7779,7 +7850,7 @@
         <xdr:cNvPr id="6" name="Gráfico 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40713AB6-5967-B5B1-1DC7-9EE3D6FCB79F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7815,7 +7886,7 @@
         <xdr:cNvPr id="7" name="Gráfico 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E263EBF5-3522-0E4A-E16B-125D347AA600}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7831,6 +7902,61 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>593911</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>105754</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95927774-837C-53F5-2388-E2F5CD150525}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9670676" cy="5439754"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -17502,488 +17628,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FDA3A2DE-A427-4D58-A9A7-F47181185571}" name="TotalSales" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="D2:E3" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="16">
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
-    <pivotField dataField="1" numFmtId="165" showAll="0"/>
-    <pivotField dataField="1" numFmtId="165" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="32">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="4"/>
-        <item x="26"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="22"/>
-        <item x="29"/>
-        <item x="17"/>
-        <item x="23"/>
-        <item x="30"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="27"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="28"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="13">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Soma de Total Selling Value" fld="12" baseField="0" baseItem="0"/>
-    <dataField name="Soma de Total Buying Value" fld="11" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{66E3FC50-82A3-42A4-BCDC-7AE80126ED5D}" name="Categorywise" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Category">
-  <location ref="AC2:AD7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
-    <pivotField dataField="1" numFmtId="165" showAll="0"/>
-    <pivotField showAll="0">
-      <items count="32">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="4"/>
-        <item x="26"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="22"/>
-        <item x="29"/>
-        <item x="17"/>
-        <item x="23"/>
-        <item x="30"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="27"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="28"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="13">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="7"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Soma de Total Selling Value" fld="12" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2662366F-2D74-4B73-8EED-17F9E7AF4544}" name="Daily" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A2:B33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="4">
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
-    <pivotField numFmtId="165" showAll="0"/>
-    <pivotField dataField="1" numFmtId="165" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="32">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="4"/>
-        <item x="26"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="22"/>
-        <item x="29"/>
-        <item x="17"/>
-        <item x="23"/>
-        <item x="30"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="27"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="28"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="13">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="13"/>
-  </rowFields>
-  <rowItems count="31">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Soma de Total Selling Value" fld="12" baseField="0" baseItem="0" numFmtId="165"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{11995CE8-2F23-4F9D-944D-5BD3B9118A70}" name="Monthly" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G2:I14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
@@ -18142,7 +17786,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CBECD968-6E96-4C08-9A79-2985EB377832}" name="Productwise" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Products">
   <location ref="P2:R46" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
@@ -18452,7 +18096,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{519FFAEF-4180-44DD-A6C6-E34FB3FED936}" name="PaymentMode" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Payment Mode">
   <location ref="AM2:AN4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
@@ -18560,12 +18204,36 @@
   <dataFields count="1">
     <dataField name="Soma de Total Selling Value" fld="12" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="1">
+  <chartFormats count="3">
     <chartFormat chart="1" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -18583,7 +18251,266 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FDA3A2DE-A427-4D58-A9A7-F47181185571}" name="TotalSales" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D2:E3" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="16">
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField dataField="1" numFmtId="165" showAll="0"/>
+    <pivotField dataField="1" numFmtId="165" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="32">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="4"/>
+        <item x="26"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="22"/>
+        <item x="29"/>
+        <item x="17"/>
+        <item x="23"/>
+        <item x="30"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="27"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="28"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Soma de Total Selling Value" fld="12" baseField="0" baseItem="0"/>
+    <dataField name="Soma de Total Buying Value" fld="11" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{66E3FC50-82A3-42A4-BCDC-7AE80126ED5D}" name="Categorywise" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Category">
+  <location ref="AC2:AD7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField dataField="1" numFmtId="165" showAll="0"/>
+    <pivotField showAll="0">
+      <items count="32">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="4"/>
+        <item x="26"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="22"/>
+        <item x="29"/>
+        <item x="17"/>
+        <item x="23"/>
+        <item x="30"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="27"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="28"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Soma de Total Selling Value" fld="12" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{37209809-68D4-4FE2-96E2-958E723714A6}" name="SalesType" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Sale Type">
   <location ref="AJ2:AK5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
@@ -18694,8 +18621,267 @@
   <dataFields count="1">
     <dataField name="Soma de Total Selling Value" fld="12" baseField="0" baseItem="0"/>
   </dataFields>
+  <chartFormats count="4">
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2662366F-2D74-4B73-8EED-17F9E7AF4544}" name="Daily" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A2:B33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField dataField="1" numFmtId="165" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="32">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="4"/>
+        <item x="26"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="22"/>
+        <item x="29"/>
+        <item x="17"/>
+        <item x="23"/>
+        <item x="30"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="27"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="28"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="13"/>
+  </rowFields>
+  <rowItems count="31">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Soma de Total Selling Value" fld="12" baseField="0" baseItem="0" numFmtId="165"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="27">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
   <chartFormats count="1">
-    <chartFormat chart="1" format="0" series="1">
+    <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -18823,46 +19009,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60351B27-4213-4B50-AF1E-6DD234ED1CD8}" name="InputData" displayName="InputData" ref="A1:P528" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60351B27-4213-4B50-AF1E-6DD234ED1CD8}" name="InputData" displayName="InputData" ref="A1:P528" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25">
   <autoFilter ref="A1:P528" xr:uid="{60351B27-4213-4B50-AF1E-6DD234ED1CD8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E527">
     <sortCondition ref="A1:A527"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{7E2D9722-C99A-4D79-AD8A-A4AF24D31B15}" name="DATE" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{1B687DA1-746A-409E-8132-464ADA2D65F7}" name="PRODUCT ID" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{3D21C161-3520-4EEB-95C2-BC89A67F811B}" name="QUANTITY" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{51AFA112-3989-4C7A-B537-003512753602}" name="SALE TYPE" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{057B8FDA-60FB-4816-999C-2030B688B9CF}" name="PAYMENT MODE" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{A77A9445-20AF-4122-92EB-C3706E536AB4}" name="DISCOUNT %" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{EF36F582-8243-4D11-B1F9-3365747E3A15}" name="PRODUCT" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{7E2D9722-C99A-4D79-AD8A-A4AF24D31B15}" name="DATE" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{1B687DA1-746A-409E-8132-464ADA2D65F7}" name="PRODUCT ID" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{3D21C161-3520-4EEB-95C2-BC89A67F811B}" name="QUANTITY" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{51AFA112-3989-4C7A-B537-003512753602}" name="SALE TYPE" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{057B8FDA-60FB-4816-999C-2030B688B9CF}" name="PAYMENT MODE" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{A77A9445-20AF-4122-92EB-C3706E536AB4}" name="DISCOUNT %" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{EF36F582-8243-4D11-B1F9-3365747E3A15}" name="PRODUCT" dataDxfId="18">
       <calculatedColumnFormula>VLOOKUP(InputData[[#This Row],[PRODUCT ID]],'Master Data'!A:B,2,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6C40EFE4-B06B-4022-A9DE-1DF212ACE9CD}" name="CATEGORY" dataDxfId="18">
+    <tableColumn id="8" xr3:uid="{6C40EFE4-B06B-4022-A9DE-1DF212ACE9CD}" name="CATEGORY" dataDxfId="17">
       <calculatedColumnFormula>VLOOKUP(InputData[[#This Row],[PRODUCT ID]],'Master Data'!A:C,3,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C0221F36-9183-46D8-9832-D4F491DFDBDF}" name="UOM" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{C0221F36-9183-46D8-9832-D4F491DFDBDF}" name="UOM" dataDxfId="16">
       <calculatedColumnFormula>VLOOKUP(InputData[[#This Row],[PRODUCT ID]],'Master Data'!A:D,4,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E273685E-A284-42EC-AECF-34BEF471CB6C}" name="BUYING PRIZE" dataDxfId="16">
+    <tableColumn id="10" xr3:uid="{E273685E-A284-42EC-AECF-34BEF471CB6C}" name="BUYING PRIZE" dataDxfId="15">
       <calculatedColumnFormula>VLOOKUP(InputData[[#This Row],[PRODUCT ID]],'Master Data'!A:E,5,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{68C3D957-3ED6-47AF-B6A5-93285DAE1B74}" name="SELLING PRICE" dataDxfId="15">
+    <tableColumn id="11" xr3:uid="{68C3D957-3ED6-47AF-B6A5-93285DAE1B74}" name="SELLING PRICE" dataDxfId="14">
       <calculatedColumnFormula>VLOOKUP(InputData[[#This Row],[PRODUCT ID]],'Master Data'!A:F,6,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{B924AB12-DCC9-42A1-8327-F9F17EBBACD1}" name="Total Buying Value" dataDxfId="14">
+    <tableColumn id="12" xr3:uid="{B924AB12-DCC9-42A1-8327-F9F17EBBACD1}" name="Total Buying Value" dataDxfId="13">
       <calculatedColumnFormula>InputData[[#This Row],[BUYING PRIZE]]*InputData[[#This Row],[QUANTITY]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F93AF158-233E-4DFA-A672-B002567615A3}" name="Total Selling Value" dataDxfId="13">
+    <tableColumn id="13" xr3:uid="{F93AF158-233E-4DFA-A672-B002567615A3}" name="Total Selling Value" dataDxfId="12">
       <calculatedColumnFormula>InputData[[#This Row],[SELLING PRICE]]*InputData[[#This Row],[QUANTITY]]*(1-InputData[[#This Row],[DISCOUNT %]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{50889A8C-3CB3-4832-B011-4EDEFF510D7D}" name="Day" dataDxfId="12">
+    <tableColumn id="14" xr3:uid="{50889A8C-3CB3-4832-B011-4EDEFF510D7D}" name="Day" dataDxfId="11">
       <calculatedColumnFormula>DAY(InputData[[#This Row],[DATE]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{DF37A157-BAFE-4A6F-8357-3A2FFB713586}" name="Month" dataDxfId="11">
+    <tableColumn id="15" xr3:uid="{DF37A157-BAFE-4A6F-8357-3A2FFB713586}" name="Month" dataDxfId="10">
       <calculatedColumnFormula>MONTH(InputData[[#This Row],[DATE]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{7A3DA93E-A613-45D1-A85F-A17814534C29}" name="Year" dataDxfId="10">
+    <tableColumn id="16" xr3:uid="{7A3DA93E-A613-45D1-A85F-A17814534C29}" name="Year" dataDxfId="9">
       <calculatedColumnFormula>YEAR(InputData[[#This Row],[DATE]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -18871,15 +19057,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DE6FA1E2-6EE8-430A-AF62-020400F3E926}" name="MasterData" displayName="MasterData" ref="A1:F46" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DE6FA1E2-6EE8-430A-AF62-020400F3E926}" name="MasterData" displayName="MasterData" ref="A1:F46" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
   <autoFilter ref="A1:F46" xr:uid="{DE6FA1E2-6EE8-430A-AF62-020400F3E926}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{106E50BA-9FFB-484D-AC75-176578AFED44}" name="PRODUCT ID" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{C6063C4C-22AC-43C3-B630-5C0916CFA263}" name="PRODUCT" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{FEA9A0A4-A0D7-45FA-BD75-4D9EBBD09441}" name="CATEGORY" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{3BDFD3DA-79CD-4B0E-9F98-1F406523093B}" name="UOM" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{C286276F-25D5-4D9D-9759-32EF67A133BE}" name="BUYING PRIZE" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{BFC92544-6510-4B40-ABEE-FD6A4B0302D7}" name="SELLING PRICE" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{106E50BA-9FFB-484D-AC75-176578AFED44}" name="PRODUCT ID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{C6063C4C-22AC-43C3-B630-5C0916CFA263}" name="PRODUCT" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{FEA9A0A4-A0D7-45FA-BD75-4D9EBBD09441}" name="CATEGORY" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{3BDFD3DA-79CD-4B0E-9F98-1F406523093B}" name="UOM" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{C286276F-25D5-4D9D-9759-32EF67A133BE}" name="BUYING PRIZE" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{BFC92544-6510-4B40-ABEE-FD6A4B0302D7}" name="SELLING PRICE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -19187,7 +19373,7 @@
   </sheetPr>
   <dimension ref="A1:AN46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -19206,8 +19392,8 @@
     <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="26" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -19310,10 +19496,10 @@
       <c r="R2" t="s">
         <v>122</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="S2" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="T2" s="15" t="s">
         <v>129</v>
       </c>
       <c r="AC2" s="9" t="s">
@@ -19342,19 +19528,19 @@
       <c r="B3" s="8">
         <v>13167.810000000001</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3">
         <v>401411.91999999969</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3">
         <v>332504</v>
       </c>
       <c r="G3" s="10">
         <v>1</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3">
         <v>34290</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3">
         <v>41346.959999999992</v>
       </c>
       <c r="K3" s="10">
@@ -19375,17 +19561,17 @@
       <c r="P3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="14">
+      <c r="Q3">
         <v>9764.7199999999993</v>
       </c>
-      <c r="R3" s="14">
+      <c r="R3">
         <v>94</v>
       </c>
-      <c r="S3" s="15">
+      <c r="S3" s="14">
         <f ca="1">RANK(V3,_xlfn.ANCHORARRAY($V$3))</f>
         <v>19</v>
       </c>
-      <c r="T3" s="16" cm="1">
+      <c r="T3" s="15" cm="1">
         <f t="array" aca="1" ref="T3:T46" ca="1">RANK(_xlfn.ANCHORARRAY(V3),_xlfn.ANCHORARRAY(V3))</f>
         <v>19</v>
       </c>
@@ -19416,10 +19602,10 @@
       <c r="AC3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AD3" s="14">
+      <c r="AD3">
         <v>69261.950000000012</v>
       </c>
-      <c r="AE3" s="14" cm="1">
+      <c r="AE3" cm="1">
         <f t="array" aca="1" ref="AE3:AE7" ca="1">RANK(_xlfn.ANCHORARRAY(AG3),_xlfn.ANCHORARRAY(AG3))</f>
         <v>4</v>
       </c>
@@ -19431,17 +19617,16 @@
         <f t="array" aca="1" ref="AG3:AG7" ca="1">OFFSET($AC$2,1,1,COUNT($AD:$AD))</f>
         <v>69261.950000000012</v>
       </c>
-      <c r="AH3" s="14"/>
       <c r="AJ3" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AK3" s="14">
+      <c r="AK3">
         <v>208140.15000000005</v>
       </c>
       <c r="AM3" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="AN3" s="14">
+      <c r="AN3">
         <v>199516.90000000008</v>
       </c>
     </row>
@@ -19455,10 +19640,10 @@
       <c r="G4" s="10">
         <v>2</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4">
         <v>25341</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4">
         <v>30857.300000000003</v>
       </c>
       <c r="K4" s="10">
@@ -19479,17 +19664,17 @@
       <c r="P4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="14">
+      <c r="Q4">
         <v>13423.199999999999</v>
       </c>
-      <c r="R4" s="14">
+      <c r="R4">
         <v>94</v>
       </c>
-      <c r="S4" s="15">
+      <c r="S4" s="14">
         <f t="shared" ref="S4:S46" ca="1" si="3">RANK(V4,_xlfn.ANCHORARRAY($V$3))</f>
         <v>10</v>
       </c>
-      <c r="T4" s="16">
+      <c r="T4" s="15">
         <f ca="1"/>
         <v>10</v>
       </c>
@@ -19520,14 +19705,14 @@
       <c r="AC4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AD4" s="14">
+      <c r="AD4">
         <v>92963.87</v>
       </c>
-      <c r="AE4" s="14">
+      <c r="AE4">
         <f ca="1"/>
         <v>2</v>
       </c>
-      <c r="AF4" s="14" t="str">
+      <c r="AF4" t="str">
         <f ca="1"/>
         <v>Category02</v>
       </c>
@@ -19535,17 +19720,16 @@
         <f ca="1"/>
         <v>92963.87</v>
       </c>
-      <c r="AH4" s="14"/>
       <c r="AJ4" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="AK4" s="14">
+      <c r="AK4">
         <v>133923.87000000002</v>
       </c>
       <c r="AM4" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="AN4" s="14">
+      <c r="AN4">
         <v>201895.01999999993</v>
       </c>
     </row>
@@ -19559,10 +19743,10 @@
       <c r="G5" s="10">
         <v>3</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5">
         <v>23437</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5">
         <v>28616.65</v>
       </c>
       <c r="K5" s="10">
@@ -19583,17 +19767,17 @@
       <c r="P5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="14">
+      <c r="Q5">
         <v>6394.2599999999993</v>
       </c>
-      <c r="R5" s="14">
+      <c r="R5">
         <v>79</v>
       </c>
-      <c r="S5" s="15">
+      <c r="S5" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>26</v>
       </c>
-      <c r="T5" s="16">
+      <c r="T5" s="15">
         <f ca="1"/>
         <v>26</v>
       </c>
@@ -19624,14 +19808,14 @@
       <c r="AC5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="AD5" s="14">
+      <c r="AD5">
         <v>52299.509999999995</v>
       </c>
-      <c r="AE5" s="14">
+      <c r="AE5">
         <f ca="1"/>
         <v>5</v>
       </c>
-      <c r="AF5" s="14" t="str">
+      <c r="AF5" t="str">
         <f ca="1"/>
         <v>Category03</v>
       </c>
@@ -19639,11 +19823,10 @@
         <f ca="1"/>
         <v>52299.509999999995</v>
       </c>
-      <c r="AH5" s="14"/>
       <c r="AJ5" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AK5" s="14">
+      <c r="AK5">
         <v>59347.900000000009</v>
       </c>
     </row>
@@ -19657,10 +19840,10 @@
       <c r="G6" s="10">
         <v>4</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6">
         <v>21282</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6">
         <v>26579.11</v>
       </c>
       <c r="K6" s="10">
@@ -19681,17 +19864,17 @@
       <c r="P6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="14">
+      <c r="Q6">
         <v>6056.1600000000008</v>
       </c>
-      <c r="R6" s="14">
+      <c r="R6">
         <v>124</v>
       </c>
-      <c r="S6" s="15">
+      <c r="S6" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>30</v>
       </c>
-      <c r="T6" s="16">
+      <c r="T6" s="15">
         <f ca="1"/>
         <v>30</v>
       </c>
@@ -19722,14 +19905,14 @@
       <c r="AC6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="AD6" s="14">
+      <c r="AD6">
         <v>95269.4</v>
       </c>
-      <c r="AE6" s="14">
+      <c r="AE6">
         <f ca="1"/>
         <v>1</v>
       </c>
-      <c r="AF6" s="14" t="str">
+      <c r="AF6" t="str">
         <f ca="1"/>
         <v>Category04</v>
       </c>
@@ -19737,7 +19920,6 @@
         <f ca="1"/>
         <v>95269.4</v>
       </c>
-      <c r="AH6" s="14"/>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -19749,10 +19931,10 @@
       <c r="G7" s="10">
         <v>5</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7">
         <v>26526</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7">
         <v>30910.45</v>
       </c>
       <c r="K7" s="10">
@@ -19773,17 +19955,17 @@
       <c r="P7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Q7" s="14">
+      <c r="Q7">
         <v>15716.61</v>
       </c>
-      <c r="R7" s="14">
+      <c r="R7">
         <v>101</v>
       </c>
-      <c r="S7" s="15">
+      <c r="S7" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>8</v>
       </c>
-      <c r="T7" s="16">
+      <c r="T7" s="15">
         <f ca="1"/>
         <v>8</v>
       </c>
@@ -19814,14 +19996,14 @@
       <c r="AC7" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="AD7" s="14">
+      <c r="AD7">
         <v>91617.19</v>
       </c>
-      <c r="AE7" s="14">
+      <c r="AE7">
         <f ca="1"/>
         <v>3</v>
       </c>
-      <c r="AF7" s="14" t="str">
+      <c r="AF7" t="str">
         <f ca="1"/>
         <v>Category05</v>
       </c>
@@ -19829,7 +20011,6 @@
         <f ca="1"/>
         <v>91617.19</v>
       </c>
-      <c r="AH7" s="14"/>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
@@ -19841,10 +20022,10 @@
       <c r="G8" s="10">
         <v>6</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8">
         <v>24879</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8">
         <v>30533.710000000003</v>
       </c>
       <c r="K8" s="10">
@@ -19865,17 +20046,17 @@
       <c r="P8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="14">
+      <c r="Q8">
         <v>4531.5</v>
       </c>
-      <c r="R8" s="14">
+      <c r="R8">
         <v>53</v>
       </c>
-      <c r="S8" s="15">
+      <c r="S8" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>35</v>
       </c>
-      <c r="T8" s="16">
+      <c r="T8" s="15">
         <f ca="1"/>
         <v>35</v>
       </c>
@@ -19914,10 +20095,10 @@
       <c r="G9" s="10">
         <v>7</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9">
         <v>29878</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9">
         <v>35251.79</v>
       </c>
       <c r="K9" s="10">
@@ -19938,17 +20119,17 @@
       <c r="P9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="Q9" s="14">
+      <c r="Q9">
         <v>2291.04</v>
       </c>
-      <c r="R9" s="14">
+      <c r="R9">
         <v>48</v>
       </c>
-      <c r="S9" s="15">
+      <c r="S9" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>39</v>
       </c>
-      <c r="T9" s="16">
+      <c r="T9" s="15">
         <f ca="1"/>
         <v>39</v>
       </c>
@@ -19987,10 +20168,10 @@
       <c r="G10" s="10">
         <v>8</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10">
         <v>29831</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10">
         <v>35350.400000000016</v>
       </c>
       <c r="K10" s="10">
@@ -20011,17 +20192,17 @@
       <c r="P10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Q10" s="14">
+      <c r="Q10">
         <v>10502.82</v>
       </c>
-      <c r="R10" s="14">
+      <c r="R10">
         <v>111</v>
       </c>
-      <c r="S10" s="15">
+      <c r="S10" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>15</v>
       </c>
-      <c r="T10" s="16">
+      <c r="T10" s="15">
         <f ca="1"/>
         <v>15</v>
       </c>
@@ -20060,10 +20241,10 @@
       <c r="G11" s="10">
         <v>9</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11">
         <v>28758</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11">
         <v>35242.810000000005</v>
       </c>
       <c r="K11" s="10">
@@ -20084,17 +20265,17 @@
       <c r="P11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="Q11" s="14">
+      <c r="Q11">
         <v>581.64</v>
       </c>
-      <c r="R11" s="14">
+      <c r="R11">
         <v>74</v>
       </c>
-      <c r="S11" s="15">
+      <c r="S11" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>44</v>
       </c>
-      <c r="T11" s="16">
+      <c r="T11" s="15">
         <f ca="1"/>
         <v>44</v>
       </c>
@@ -20133,10 +20314,10 @@
       <c r="G12" s="10">
         <v>10</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12">
         <v>27842</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12">
         <v>33500.69000000001</v>
       </c>
       <c r="K12" s="10">
@@ -20157,17 +20338,17 @@
       <c r="P12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="Q12" s="14">
+      <c r="Q12">
         <v>16428</v>
       </c>
-      <c r="R12" s="14">
+      <c r="R12">
         <v>100</v>
       </c>
-      <c r="S12" s="15">
+      <c r="S12" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>5</v>
       </c>
-      <c r="T12" s="16">
+      <c r="T12" s="15">
         <f ca="1"/>
         <v>5</v>
       </c>
@@ -20206,10 +20387,10 @@
       <c r="G13" s="10">
         <v>11</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13">
         <v>29306</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13">
         <v>36124.07</v>
       </c>
       <c r="K13" s="10">
@@ -20230,17 +20411,17 @@
       <c r="P13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="Q13" s="14">
+      <c r="Q13">
         <v>5856.4</v>
       </c>
-      <c r="R13" s="14">
+      <c r="R13">
         <v>121</v>
       </c>
-      <c r="S13" s="15">
+      <c r="S13" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>31</v>
       </c>
-      <c r="T13" s="16">
+      <c r="T13" s="15">
         <f ca="1"/>
         <v>31</v>
       </c>
@@ -20267,10 +20448,10 @@
       <c r="G14" s="10">
         <v>12</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14">
         <v>31134</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14">
         <v>37097.979999999996</v>
       </c>
       <c r="K14" s="10">
@@ -20291,17 +20472,17 @@
       <c r="P14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="Q14" s="14">
+      <c r="Q14">
         <v>11582.910000000003</v>
       </c>
-      <c r="R14" s="14">
+      <c r="R14">
         <v>123</v>
       </c>
-      <c r="S14" s="15">
+      <c r="S14" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>13</v>
       </c>
-      <c r="T14" s="16">
+      <c r="T14" s="15">
         <f ca="1"/>
         <v>13</v>
       </c>
@@ -20328,17 +20509,17 @@
       <c r="P15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="Q15" s="14">
+      <c r="Q15">
         <v>8423.52</v>
       </c>
-      <c r="R15" s="14">
+      <c r="R15">
         <v>69</v>
       </c>
-      <c r="S15" s="15">
+      <c r="S15" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>22</v>
       </c>
-      <c r="T15" s="16">
+      <c r="T15" s="15">
         <f ca="1"/>
         <v>22</v>
       </c>
@@ -20372,17 +20553,17 @@
       <c r="P16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="Q16" s="14">
+      <c r="Q16">
         <v>12764.640000000001</v>
       </c>
-      <c r="R16" s="14">
+      <c r="R16">
         <v>87</v>
       </c>
-      <c r="S16" s="15">
+      <c r="S16" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>12</v>
       </c>
-      <c r="T16" s="16">
+      <c r="T16" s="15">
         <f ca="1"/>
         <v>12</v>
       </c>
@@ -20416,17 +20597,17 @@
       <c r="P17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="Q17" s="14">
+      <c r="Q17">
         <v>1839.2399999999998</v>
       </c>
-      <c r="R17" s="14">
+      <c r="R17">
         <v>117</v>
       </c>
-      <c r="S17" s="15">
+      <c r="S17" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>41</v>
       </c>
-      <c r="T17" s="16">
+      <c r="T17" s="15">
         <f ca="1"/>
         <v>41</v>
       </c>
@@ -20460,17 +20641,17 @@
       <c r="P18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="Q18" s="14">
+      <c r="Q18">
         <v>1996.8</v>
       </c>
-      <c r="R18" s="14">
+      <c r="R18">
         <v>120</v>
       </c>
-      <c r="S18" s="15">
+      <c r="S18" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>40</v>
       </c>
-      <c r="T18" s="16">
+      <c r="T18" s="15">
         <f ca="1"/>
         <v>40</v>
       </c>
@@ -20497,17 +20678,17 @@
       <c r="P19" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="Q19" s="14">
+      <c r="Q19">
         <v>9877.1400000000012</v>
       </c>
-      <c r="R19" s="14">
+      <c r="R19">
         <v>63</v>
       </c>
-      <c r="S19" s="15">
+      <c r="S19" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>18</v>
       </c>
-      <c r="T19" s="16">
+      <c r="T19" s="15">
         <f ca="1"/>
         <v>18</v>
       </c>
@@ -20534,17 +20715,17 @@
       <c r="P20" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="Q20" s="14">
+      <c r="Q20">
         <v>4035.2200000000003</v>
       </c>
-      <c r="R20" s="14">
+      <c r="R20">
         <v>82</v>
       </c>
-      <c r="S20" s="15">
+      <c r="S20" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>36</v>
       </c>
-      <c r="T20" s="16">
+      <c r="T20" s="15">
         <f ca="1"/>
         <v>36</v>
       </c>
@@ -20571,17 +20752,17 @@
       <c r="P21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="Q21" s="14">
+      <c r="Q21">
         <v>20160</v>
       </c>
-      <c r="R21" s="14">
+      <c r="R21">
         <v>96</v>
       </c>
-      <c r="S21" s="15">
+      <c r="S21" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>4</v>
       </c>
-      <c r="T21" s="16">
+      <c r="T21" s="15">
         <f ca="1"/>
         <v>4</v>
       </c>
@@ -20608,17 +20789,17 @@
       <c r="P22" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="Q22" s="14">
+      <c r="Q22">
         <v>8006.25</v>
       </c>
-      <c r="R22" s="14">
+      <c r="R22">
         <v>105</v>
       </c>
-      <c r="S22" s="15">
+      <c r="S22" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>23</v>
       </c>
-      <c r="T22" s="16">
+      <c r="T22" s="15">
         <f ca="1"/>
         <v>23</v>
       </c>
@@ -20645,17 +20826,17 @@
       <c r="P23" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="Q23" s="14">
+      <c r="Q23">
         <v>10727.64</v>
       </c>
-      <c r="R23" s="14">
+      <c r="R23">
         <v>66</v>
       </c>
-      <c r="S23" s="15">
+      <c r="S23" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>14</v>
       </c>
-      <c r="T23" s="16">
+      <c r="T23" s="15">
         <f ca="1"/>
         <v>14</v>
       </c>
@@ -20682,17 +20863,17 @@
       <c r="P24" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="Q24" s="14">
+      <c r="Q24">
         <v>9909.9</v>
       </c>
-      <c r="R24" s="14">
+      <c r="R24">
         <v>70</v>
       </c>
-      <c r="S24" s="15">
+      <c r="S24" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>17</v>
       </c>
-      <c r="T24" s="16">
+      <c r="T24" s="15">
         <f ca="1"/>
         <v>17</v>
       </c>
@@ -20719,17 +20900,17 @@
       <c r="P25" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="Q25" s="14">
+      <c r="Q25">
         <v>12853.560000000001</v>
       </c>
-      <c r="R25" s="14">
+      <c r="R25">
         <v>86</v>
       </c>
-      <c r="S25" s="15">
+      <c r="S25" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>11</v>
       </c>
-      <c r="T25" s="16">
+      <c r="T25" s="15">
         <f ca="1"/>
         <v>11</v>
       </c>
@@ -20756,17 +20937,17 @@
       <c r="P26" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="Q26" s="14">
+      <c r="Q26">
         <v>10202.400000000001</v>
       </c>
-      <c r="R26" s="14">
+      <c r="R26">
         <v>65</v>
       </c>
-      <c r="S26" s="15">
+      <c r="S26" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>16</v>
       </c>
-      <c r="T26" s="16">
+      <c r="T26" s="15">
         <f ca="1"/>
         <v>16</v>
       </c>
@@ -20793,17 +20974,17 @@
       <c r="P27" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="Q27" s="14">
+      <c r="Q27">
         <v>599.7600000000001</v>
       </c>
-      <c r="R27" s="14">
+      <c r="R27">
         <v>72</v>
       </c>
-      <c r="S27" s="15">
+      <c r="S27" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>43</v>
       </c>
-      <c r="T27" s="16">
+      <c r="T27" s="15">
         <f ca="1"/>
         <v>43</v>
       </c>
@@ -20830,17 +21011,17 @@
       <c r="P28" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="Q28" s="14">
+      <c r="Q28">
         <v>2761.9200000000005</v>
       </c>
-      <c r="R28" s="14">
+      <c r="R28">
         <v>112</v>
       </c>
-      <c r="S28" s="15">
+      <c r="S28" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>38</v>
       </c>
-      <c r="T28" s="16">
+      <c r="T28" s="15">
         <f ca="1"/>
         <v>38</v>
       </c>
@@ -20867,17 +21048,17 @@
       <c r="P29" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="Q29" s="14">
+      <c r="Q29">
         <v>6226.0800000000008</v>
       </c>
-      <c r="R29" s="14">
+      <c r="R29">
         <v>109</v>
       </c>
-      <c r="S29" s="15">
+      <c r="S29" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>28</v>
       </c>
-      <c r="T29" s="16">
+      <c r="T29" s="15">
         <f ca="1"/>
         <v>28</v>
       </c>
@@ -20904,17 +21085,17 @@
       <c r="P30" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="Q30" s="14">
+      <c r="Q30">
         <v>4682.72</v>
       </c>
-      <c r="R30" s="14">
+      <c r="R30">
         <v>112</v>
       </c>
-      <c r="S30" s="15">
+      <c r="S30" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>34</v>
       </c>
-      <c r="T30" s="16">
+      <c r="T30" s="15">
         <f ca="1"/>
         <v>34</v>
       </c>
@@ -20941,17 +21122,17 @@
       <c r="P31" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="Q31" s="14">
+      <c r="Q31">
         <v>5523.44</v>
       </c>
-      <c r="R31" s="14">
+      <c r="R31">
         <v>104</v>
       </c>
-      <c r="S31" s="15">
+      <c r="S31" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>32</v>
       </c>
-      <c r="T31" s="16">
+      <c r="T31" s="15">
         <f ca="1"/>
         <v>32</v>
       </c>
@@ -20978,17 +21159,17 @@
       <c r="P32" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="Q32" s="14">
+      <c r="Q32">
         <v>22945.919999999998</v>
       </c>
-      <c r="R32" s="14">
+      <c r="R32">
         <v>114</v>
       </c>
-      <c r="S32" s="15">
+      <c r="S32" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>2</v>
       </c>
-      <c r="T32" s="16">
+      <c r="T32" s="15">
         <f ca="1"/>
         <v>2</v>
       </c>
@@ -21015,17 +21196,17 @@
       <c r="P33" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="Q33" s="14">
+      <c r="Q33">
         <v>6249.5999999999995</v>
       </c>
-      <c r="R33" s="14">
+      <c r="R33">
         <v>60</v>
       </c>
-      <c r="S33" s="15">
+      <c r="S33" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>27</v>
       </c>
-      <c r="T33" s="16">
+      <c r="T33" s="15">
         <f ca="1"/>
         <v>27</v>
       </c>
@@ -21046,17 +21227,17 @@
       <c r="P34" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="Q34" s="14">
+      <c r="Q34">
         <v>16329.72</v>
       </c>
-      <c r="R34" s="14">
+      <c r="R34">
         <v>139</v>
       </c>
-      <c r="S34" s="15">
+      <c r="S34" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>7</v>
       </c>
-      <c r="T34" s="16">
+      <c r="T34" s="15">
         <f ca="1"/>
         <v>7</v>
       </c>
@@ -21077,17 +21258,17 @@
       <c r="P35" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="Q35" s="14">
+      <c r="Q35">
         <v>13645.800000000001</v>
       </c>
-      <c r="R35" s="14">
+      <c r="R35">
         <v>114</v>
       </c>
-      <c r="S35" s="15">
+      <c r="S35" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>9</v>
       </c>
-      <c r="T35" s="16">
+      <c r="T35" s="15">
         <f ca="1"/>
         <v>9</v>
       </c>
@@ -21108,17 +21289,17 @@
       <c r="P36" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="Q36" s="14">
+      <c r="Q36">
         <v>8978.2000000000007</v>
       </c>
-      <c r="R36" s="14">
+      <c r="R36">
         <v>154</v>
       </c>
-      <c r="S36" s="15">
+      <c r="S36" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>20</v>
       </c>
-      <c r="T36" s="16">
+      <c r="T36" s="15">
         <f ca="1"/>
         <v>20</v>
       </c>
@@ -21139,17 +21320,17 @@
       <c r="P37" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="Q37" s="14">
+      <c r="Q37">
         <v>703.5</v>
       </c>
-      <c r="R37" s="14">
+      <c r="R37">
         <v>105</v>
       </c>
-      <c r="S37" s="15">
+      <c r="S37" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>42</v>
       </c>
-      <c r="T37" s="16">
+      <c r="T37" s="15">
         <f ca="1"/>
         <v>42</v>
       </c>
@@ -21170,17 +21351,17 @@
       <c r="P38" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="Q38" s="14">
+      <c r="Q38">
         <v>7222.5</v>
       </c>
-      <c r="R38" s="14">
+      <c r="R38">
         <v>75</v>
       </c>
-      <c r="S38" s="15">
+      <c r="S38" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>25</v>
       </c>
-      <c r="T38" s="16">
+      <c r="T38" s="15">
         <f ca="1"/>
         <v>25</v>
       </c>
@@ -21201,17 +21382,17 @@
       <c r="P39" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="Q39" s="14">
+      <c r="Q39">
         <v>5145.6000000000004</v>
       </c>
-      <c r="R39" s="14">
+      <c r="R39">
         <v>60</v>
       </c>
-      <c r="S39" s="15">
+      <c r="S39" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>33</v>
       </c>
-      <c r="T39" s="16">
+      <c r="T39" s="15">
         <f ca="1"/>
         <v>33</v>
       </c>
@@ -21232,17 +21413,17 @@
       <c r="P40" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="Q40" s="14">
+      <c r="Q40">
         <v>8871.1200000000008</v>
       </c>
-      <c r="R40" s="14">
+      <c r="R40">
         <v>111</v>
       </c>
-      <c r="S40" s="15">
+      <c r="S40" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>21</v>
       </c>
-      <c r="T40" s="16">
+      <c r="T40" s="15">
         <f ca="1"/>
         <v>21</v>
       </c>
@@ -21263,17 +21444,17 @@
       <c r="P41" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="Q41" s="14">
+      <c r="Q41">
         <v>3957.15</v>
       </c>
-      <c r="R41" s="14">
+      <c r="R41">
         <v>93</v>
       </c>
-      <c r="S41" s="15">
+      <c r="S41" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>37</v>
       </c>
-      <c r="T41" s="16">
+      <c r="T41" s="15">
         <f ca="1"/>
         <v>37</v>
       </c>
@@ -21294,17 +21475,17 @@
       <c r="P42" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="Q42" s="14">
+      <c r="Q42">
         <v>7718.4000000000005</v>
       </c>
-      <c r="R42" s="14">
+      <c r="R42">
         <v>67</v>
       </c>
-      <c r="S42" s="15">
+      <c r="S42" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>24</v>
       </c>
-      <c r="T42" s="16">
+      <c r="T42" s="15">
         <f ca="1"/>
         <v>24</v>
       </c>
@@ -21325,17 +21506,17 @@
       <c r="P43" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="Q43" s="14">
+      <c r="Q43">
         <v>22952.16</v>
       </c>
-      <c r="R43" s="14">
+      <c r="R43">
         <v>132</v>
       </c>
-      <c r="S43" s="15">
+      <c r="S43" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
-      <c r="T43" s="16">
+      <c r="T43" s="15">
         <f ca="1"/>
         <v>1</v>
       </c>
@@ -21356,17 +21537,17 @@
       <c r="P44" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="Q44" s="14">
+      <c r="Q44">
         <v>20574</v>
       </c>
-      <c r="R44" s="14">
+      <c r="R44">
         <v>127</v>
       </c>
-      <c r="S44" s="15">
+      <c r="S44" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>3</v>
       </c>
-      <c r="T44" s="16">
+      <c r="T44" s="15">
         <f ca="1"/>
         <v>3</v>
       </c>
@@ -21387,17 +21568,17 @@
       <c r="P45" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="Q45" s="14">
+      <c r="Q45">
         <v>6064.8399999999992</v>
       </c>
-      <c r="R45" s="14">
+      <c r="R45">
         <v>73</v>
       </c>
-      <c r="S45" s="15">
+      <c r="S45" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>29</v>
       </c>
-      <c r="T45" s="16">
+      <c r="T45" s="15">
         <f ca="1"/>
         <v>29</v>
       </c>
@@ -21418,17 +21599,17 @@
       <c r="P46" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="Q46" s="14">
+      <c r="Q46">
         <v>16333.92</v>
       </c>
-      <c r="R46" s="14">
+      <c r="R46">
         <v>199</v>
       </c>
-      <c r="S46" s="15">
+      <c r="S46" s="14">
         <f t="shared" ca="1" si="3"/>
         <v>6</v>
       </c>
-      <c r="T46" s="16">
+      <c r="T46" s="15">
         <f ca="1"/>
         <v>6</v>
       </c>
@@ -21554,6 +21735,56 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEF8F26-A6C1-4B2D-8D53-E409D9B5AAAA}">
+  <dimension ref="A1:A30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F31" sqref="A31:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="17" width="9.140625" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" x14ac:dyDescent="0.25"/>
+    <row r="2" x14ac:dyDescent="0.25"/>
+    <row r="3" x14ac:dyDescent="0.25"/>
+    <row r="4" x14ac:dyDescent="0.25"/>
+    <row r="5" x14ac:dyDescent="0.25"/>
+    <row r="6" x14ac:dyDescent="0.25"/>
+    <row r="7" x14ac:dyDescent="0.25"/>
+    <row r="8" x14ac:dyDescent="0.25"/>
+    <row r="9" x14ac:dyDescent="0.25"/>
+    <row r="10" x14ac:dyDescent="0.25"/>
+    <row r="11" x14ac:dyDescent="0.25"/>
+    <row r="12" x14ac:dyDescent="0.25"/>
+    <row r="13" x14ac:dyDescent="0.25"/>
+    <row r="14" x14ac:dyDescent="0.25"/>
+    <row r="15" x14ac:dyDescent="0.25"/>
+    <row r="16" x14ac:dyDescent="0.25"/>
+    <row r="17" x14ac:dyDescent="0.25"/>
+    <row r="18" x14ac:dyDescent="0.25"/>
+    <row r="19" x14ac:dyDescent="0.25"/>
+    <row r="20" x14ac:dyDescent="0.25"/>
+    <row r="21" x14ac:dyDescent="0.25"/>
+    <row r="22" x14ac:dyDescent="0.25"/>
+    <row r="23" x14ac:dyDescent="0.25"/>
+    <row r="24" x14ac:dyDescent="0.25"/>
+    <row r="25" x14ac:dyDescent="0.25"/>
+    <row r="26" x14ac:dyDescent="0.25"/>
+    <row r="27" x14ac:dyDescent="0.25"/>
+    <row r="28" x14ac:dyDescent="0.25"/>
+    <row r="29" x14ac:dyDescent="0.25"/>
+    <row r="30" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B86BCA6-DF35-4AD0-B1A4-40571F66AE92}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -53272,7 +53503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C072B0D-0958-4B40-9249-FB0E3D41DBB9}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>

</xml_diff>